<commit_message>
Changement des exemples des images de evt et actu dans le dico des données
</commit_message>
<xml_diff>
--- a/competences/c4_bd/DictionnaireDonnee.xlsx
+++ b/competences/c4_bd/DictionnaireDonnee.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iutbayonne.sharepoint.com/sites/SA3.01Groupe7-GureKultura/Documents partages/General/S3/3 - Pôle gestion des données (C4)/donnees/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BACB280F-8B4B-4246-B7CB-D578C9DCF95A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{22A971EA-3777-4288-A6D6-F85721BB0C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13056" xr2:uid="{8CC2DDE9-D2EC-4C7C-A51B-5F689ABCD9FB}"/>
   </bookViews>
@@ -347,7 +347,7 @@
     <t>img</t>
   </si>
   <si>
-    <t>/images/events/pelote.jpg</t>
+    <t>pelote.jpg</t>
   </si>
   <si>
     <t>#cateId</t>
@@ -398,7 +398,7 @@
     <t xml:space="preserve">La date de publication de l’article sur le site </t>
   </si>
   <si>
-    <t>/images/actu/aviron.jpg</t>
+    <t>aviron.jpg</t>
   </si>
   <si>
     <t>Categorie</t>
@@ -1338,7 +1338,7 @@
   <dimension ref="A1:R67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>